<commit_message>
Update final version of the draft and update many pictures
</commit_message>
<xml_diff>
--- a/doc/theory_pics/Figure 3.xlsx
+++ b/doc/theory_pics/Figure 3.xlsx
@@ -12,10 +12,6 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1762,7 +1758,7 @@
           <c:max val="2"/>
           <c:min val="-2"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1782,39 +1778,6 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="413872216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -1825,7 +1788,7 @@
           <c:orientation val="minMax"/>
           <c:min val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1908,39 +1871,6 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="413871888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -2551,7 +2481,7 @@
           <c:max val="2"/>
           <c:min val="-2"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2571,39 +2501,6 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="413872216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -2614,7 +2511,7 @@
           <c:orientation val="minMax"/>
           <c:min val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2697,39 +2594,6 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="413871888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -3339,7 +3203,7 @@
           <c:max val="2"/>
           <c:min val="-2"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3359,39 +3223,6 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="413872216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -3402,7 +3233,7 @@
           <c:orientation val="minMax"/>
           <c:min val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3485,39 +3316,6 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="413871888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -7755,32 +7553,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8255,7 +8027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>